<commit_message>
updated interface and DB
</commit_message>
<xml_diff>
--- a/assets/RPP_Dataset - Copy.xlsx
+++ b/assets/RPP_Dataset - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rag-Vector-DB\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3BDA12-9855-49BD-9FD1-BDB7E9D07F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC436F7-EA1F-46E2-9D07-B8D2AA9B8F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CA81EEF-E1C1-4348-B691-E48AE177628C}"/>
   </bookViews>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24584B9-B52C-411B-BAFB-094DF5D7B5CE}">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
separate css, js, html
new interface with BG photo, with Tamil, English capability, and with feedback section
</commit_message>
<xml_diff>
--- a/assets/RPP_Dataset - Copy.xlsx
+++ b/assets/RPP_Dataset - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rag-Vector-DB\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC436F7-EA1F-46E2-9D07-B8D2AA9B8F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C34F397-C6E5-4A82-B40B-245D75C7EA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CA81EEF-E1C1-4348-B691-E48AE177628C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="152">
   <si>
     <t>Disease Name</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>dog</t>
-  </si>
-  <si>
-    <t>Panchagavya for Animal Health</t>
   </si>
   <si>
     <t>Milk fever or Calcium Deficiency</t>
@@ -619,9 +616,6 @@
 powder and apply to the wound. Repeat this application till the point of cure.</t>
   </si>
   <si>
-    <t>Panchakavya</t>
-  </si>
-  <si>
     <t>Chickens</t>
   </si>
   <si>
@@ -670,14 +664,93 @@
 thoroughly.
 Internal Medication: Administer 15 gm of Ashta Choornam internally.</t>
   </si>
+  <si>
+    <t>Panchagavya for Animal Health(infertility or repeat breeding)</t>
+  </si>
+  <si>
+    <t>Panchakavya(infertility or repeat breeding)</t>
+  </si>
+  <si>
+    <t>Fracture and broken leg</t>
+  </si>
+  <si>
+    <t>Fractures of the bone occur due to accidents or sudden fall of animals or aggression with other animals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black gram 200 gm,add 3 egg whites of country chicken ,100 ml of sesame oil ,Take tender leaves and primordial region of Asthibhanga (Cissus quadrangularis), rhizome of Ashwagandha (Withania somnifera) each 10 gm,300 ml of milk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">External medicine
+Take black gram 200 gm and made into powder and add 3 egg whites of country chicken and mix it well. This paste is to be applied on the wounded area and put bamboo sticks around the affected bone and tie it with a cotton cloth around it. After tieing it, pour 100 ml of sesame oil on the upper part of the cotton cloth. After 15 days remove the cloth and continue the same procedure 
+Internal medicine :Take tender leaves and primordial region of Asthibhanga (Cissus quadrangularis), rhizome of Ashwagandha (Withania somnifera) each 10 gm and ground them well. Add 300 ml of milk and mix it well and administered orally. </t>
+  </si>
+  <si>
+    <t>To Increase Milk</t>
+  </si>
+  <si>
+    <t>cow,goat</t>
+  </si>
+  <si>
+    <t>Bottle gourd or white coloured Pumpkin 100 gm, Coconut (grated) 100 gm, Black gram 100gm, Jaggery 100 gm. Black gram is to be soaked for overnight. It is to be ground well along with coconut, bottle gourd (chopped) and jaggery. Then the paste like substance is to be fed to the animal. It should be given once a day for 2-5 days</t>
+  </si>
+  <si>
+    <t>Fracture of horn</t>
+  </si>
+  <si>
+    <t>Occurs due to accidents, cow bumping, broken horns, due to incidence of disease etc</t>
+  </si>
+  <si>
+    <t>1. Add sugar and apply it on the affected area.
+2. Add required amount of kanphuli (Tridax procumbens) and turmeric powder and mix it in coconut oil.
+3. Dip a cotton cloth in the latex of baniyan tree or cactus Spiral spruge (Euphorbia tortilis) paste and wrap it around the area.
+4. Apply Mathaan thaila / ointment on the affected area.</t>
+  </si>
+  <si>
+    <t>sugar,kanphuli (Tridax procumbens),turmeric powder,coconut oil,baniyan tree or cactus Spiral spruge (Euphorbia tortilis),ointment</t>
+  </si>
+  <si>
+    <t>Pumpkin 100 gm, Coconut (grated) 100 gm, Black gram 100gm, Jaggery 100 gm,coconut</t>
+  </si>
+  <si>
+    <t>Cow unable to stand up or falling suddenly</t>
+  </si>
+  <si>
+    <t>The head hangs. The cow is tired and has trembling legs. The leg does not stand still, the leg bends. The forefoot is the first to be affected. Does not move. The eyes twitched. Eats soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three eggs of country chicken,curry leaves,a handful of pirandai,a handful of drumstick leaves,a handful of agathi keerai,a handful of thaluthalai,200 gm of coconut inflorescence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A handful of rock salt is placed in the tongue of animal. Take three eggs of country chicken administered orally and give them once a day for two days. Take a handful of curry leaves (Murraya koenigii), a handful of pirandai (Cissus quadrangularis), a handful of drumstick leaves (Moringa oleifera), a handful of agathi keerai (Sesbania grandiflora), a handful of thaluthalai (Clerodendrum phlomides) and 200 gm of coconut inflorescence and all are ground well together. Then mix it with ½ lit. of coconut milk and administered orally. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -704,18 +777,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24584B9-B52C-411B-BAFB-094DF5D7B5CE}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="93" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,22 +1147,22 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
@@ -1091,23 +1172,23 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="L2" t="str">
         <f t="shared" ref="L2:L3" si="0">CONCATENATE(I2,",",J2,",",K2)</f>
         <v>,,</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1122,23 +1203,23 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
         <v>,,</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1153,22 +1234,22 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
@@ -1178,22 +1259,22 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -1203,22 +1284,22 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P6" s="1"/>
     </row>
@@ -1229,22 +1310,22 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P7" s="1"/>
     </row>
@@ -1255,22 +1336,22 @@
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="C8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1283,22 +1364,22 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="L9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1311,22 +1392,22 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="L10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1339,22 +1420,22 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="L11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1367,23 +1448,23 @@
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="C12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
       <c r="L12" t="str">
         <f t="shared" ref="L12:L39" si="1">CONCATENATE(I12,",",J12,",",K12)</f>
         <v>,,</v>
       </c>
       <c r="M12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1396,23 +1477,23 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="L13" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -1425,23 +1506,23 @@
       <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="L14" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1454,23 +1535,23 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
       <c r="L15" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -1482,23 +1563,23 @@
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="C16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="L16" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -1511,23 +1592,23 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="C17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
       <c r="L17" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1540,22 +1621,22 @@
       <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="C18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="L18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -1570,22 +1651,22 @@
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="C19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="L19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -1600,22 +1681,22 @@
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="C20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="L20" t="s">
         <v>18</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P20" s="1"/>
     </row>
@@ -1626,22 +1707,22 @@
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="C21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="L21" t="s">
         <v>18</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P21" s="1"/>
     </row>
@@ -1652,21 +1733,21 @@
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="L22" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P22" s="1"/>
     </row>
@@ -1677,21 +1758,21 @@
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="L23" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P23" s="1"/>
     </row>
@@ -1702,23 +1783,23 @@
       <c r="B24" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
       <c r="L24" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1730,21 +1811,21 @@
       <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
       <c r="L25" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1756,23 +1837,23 @@
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="C26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
       <c r="L26" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -1784,23 +1865,23 @@
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="C27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
       <c r="L27" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P27" s="1"/>
     </row>
@@ -1811,23 +1892,23 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="C28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
       <c r="L28" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P28" s="1"/>
     </row>
@@ -1838,21 +1919,21 @@
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
       <c r="L29" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P29" s="1"/>
     </row>
@@ -1863,21 +1944,21 @@
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
       <c r="L30" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P30" s="1"/>
     </row>
@@ -1888,21 +1969,21 @@
       <c r="B31" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
       <c r="L31" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P31" s="1"/>
     </row>
@@ -1913,21 +1994,21 @@
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
       <c r="L32" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P32" s="1"/>
     </row>
@@ -1938,22 +2019,22 @@
       <c r="B33" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="C33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
       <c r="L33" t="s">
         <v>29</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -1963,21 +2044,21 @@
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="L34" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -1987,354 +2068,921 @@
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="L35" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="L36" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
       <c r="L37" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="I38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P38" s="1"/>
     </row>
     <row r="39" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="L39" t="str">
         <f t="shared" si="1"/>
         <v>,,</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P40" s="1"/>
     </row>
     <row r="41" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P41" s="1"/>
     </row>
     <row r="42" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
     <row r="43" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
     <row r="44" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="L44" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
         <v>116</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="L45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="L46" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="M47" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B47" t="s">
+      <c r="N47" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="M47" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="L48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="M48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="L48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>135</v>
-      </c>
+    </row>
+    <row r="49" spans="1:14" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="M49" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="M50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="M51" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="M52" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+    </row>
+    <row r="111" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C37:H37"/>
+  <mergeCells count="135">
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C50:E50"/>
     <mergeCell ref="C42:H42"/>
     <mergeCell ref="C43:H43"/>
     <mergeCell ref="C6:H6"/>
@@ -2351,16 +2999,24 @@
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C24:H24"/>
     <mergeCell ref="C26:H26"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="C28:H28"/>
@@ -2370,11 +3026,6 @@
     <mergeCell ref="C30:H30"/>
     <mergeCell ref="C31:H31"/>
     <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>